<commit_message>
Watchdog Timer funktioniert. Einige Implementierungsfragen sind jedoch noch offen (siehe Exceltabelle). Vor allem Dingen, wie man diese 18ms berechnen soll...
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Allg. Logik und TMR0 implementiert, RB0 und Rest noch nicht</t>
+  </si>
+  <si>
+    <t>in Arbeit - die Umsetzung der 18ms sind noch unklar(im Simulator abhängig von Quarzfrequenz?) + ist mit Devise Reset ein Neustart gemeint order ein Stop nach Reset? Und wtf soll ich unter dem Postscaler verstehen?</t>
   </si>
 </sst>
 </file>
@@ -498,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +717,7 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -726,7 +729,7 @@
       </c>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -738,7 +741,7 @@
       </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
@@ -748,7 +751,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>21</v>
       </c>
@@ -760,7 +763,7 @@
       </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -768,11 +771,14 @@
         <v>3</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -784,7 +790,7 @@
       </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -796,7 +802,7 @@
       </c>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -808,7 +814,7 @@
       </c>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -820,7 +826,7 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
@@ -832,7 +838,7 @@
       </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>
@@ -844,7 +850,7 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -853,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>30</v>
       </c>
@@ -865,7 +871,7 @@
       </c>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>31</v>
       </c>
@@ -876,7 +882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>32</v>
       </c>
@@ -887,7 +893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
@@ -908,7 +914,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -921,7 +927,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.73333333333333328</v>
+        <v>0.76666666666666672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Psst! Auf Bug Jagd!
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>in Arbeit - die Umsetzung der 18ms sind noch unklar(im Simulator abhängig von Quarzfrequenz?) + ist mit Devise Reset ein Neustart gemeint order ein Stop nach Reset? Und wtf soll ich unter dem Postscaler verstehen?</t>
+  </si>
+  <si>
+    <t>TODO: Einmal organisiert durchgehen</t>
   </si>
 </sst>
 </file>
@@ -501,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,6 +605,9 @@
         <v>0</v>
       </c>
       <c r="E7" s="3"/>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -614,6 +620,9 @@
         <v>0</v>
       </c>
       <c r="E8" s="3"/>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -635,9 +644,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3"/>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -914,7 +926,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -927,7 +939,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.76666666666666672</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO-Liste und Tabelle auf neuesten Stand
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -144,13 +144,13 @@
     <t>Allg. Logik und TMR0 implementiert, RB0 und Rest noch nicht</t>
   </si>
   <si>
-    <t>in Arbeit - die Umsetzung der 18ms sind noch unklar(im Simulator abhängig von Quarzfrequenz?) + ist mit Devise Reset ein Neustart gemeint order ein Stop nach Reset? Und wtf soll ich unter dem Postscaler verstehen?</t>
-  </si>
-  <si>
     <t>TODO</t>
   </si>
   <si>
     <t>TODO: Einmal organisiert durchgehen</t>
+  </si>
+  <si>
+    <t>Berechnung der gewünschten Time-Out-Periode macht immer noch keinen Sinn. Bei 200ns Zykluszeit und 18 ms gewünschtem Timeout komme ich auf 90 000 Zyklen. Lehmann fordert in SimTest04 aber aus irgendeinem Grund nur 17 949. Nochmal nachfragen</t>
   </si>
 </sst>
 </file>
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +609,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +624,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -651,7 +651,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,7 +693,7 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,11 +792,11 @@
         <v>3</v>
       </c>
       <c r="D21" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,7 +935,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -948,7 +948,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.75</v>
+        <v>0.76666666666666672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Port B Interrupt vollständig - 80% der benötigten Punkte
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>externer Takt? Muss das im Simulator erzeugt werden oder ist Nutzereingabe ausreichend?</t>
-  </si>
-  <si>
-    <t>Allg. Logik und TMR0 implementiert, RB0 und Rest noch nicht</t>
   </si>
   <si>
     <t>TODO</t>
@@ -508,7 +505,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +606,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -624,7 +621,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -651,7 +648,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,7 +690,7 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,12 +713,9 @@
         <v>5</v>
       </c>
       <c r="D15" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -759,7 +753,7 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,7 +790,7 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,7 +929,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -948,7 +942,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.76666666666666672</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PCLATH abgeschlossen - I'll be back!
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
84% - EEPROM Funktionalität - SimTest09 funktioniert aber nur zur Hälfte (Bug bei Read)
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Berechnung der gewünschten Time-Out-Periode macht immer noch keinen Sinn. Bei 200ns Zykluszeit und 18 ms gewünschtem Timeout komme ich auf 90 000 Zyklen. Lehmann fordert in SimTest04 aber aus irgendeinem Grund nur 17 949. Nochmal nachfragen</t>
+  </si>
+  <si>
+    <t>TODO: Bug bei Read</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,9 +777,12 @@
         <v>5</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E20" s="3"/>
+      <c r="F20" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
@@ -929,7 +935,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>48</v>
+        <v>50.5</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -942,7 +948,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.8</v>
+        <v>0.84166666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checkliste und Todo Update
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" t="s">
@@ -929,7 +929,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -942,7 +942,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.8833333333333333</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO und Tabelle Update
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,12 +686,9 @@
         <v>2</v>
       </c>
       <c r="D13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -825,7 +822,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -929,7 +926,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -942,7 +939,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.91666666666666663</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
92% - SLEEP Funktion
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
   <si>
     <t>Punkte gesamt</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Berechnung der gewünschten Time-Out-Periode macht immer noch keinen Sinn. Bei 200ns Zykluszeit und 18 ms gewünschtem Timeout komme ich auf 90 000 Zyklen. Lehmann fordert in SimTest04 aber aus irgendeinem Grund nur 17 949. Nochmal nachfragen</t>
+  </si>
+  <si>
+    <t>Hält sich noch nicht ganz an die Beschreibung (WakeUps sind manuell gesetzt, die RESETs bewirken irgendwie so gut wie nichts…)</t>
   </si>
 </sst>
 </file>
@@ -504,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -798,9 +801,12 @@
         <v>3</v>
       </c>
       <c r="D22" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3"/>
+      <c r="F22" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
@@ -926,7 +932,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -939,7 +945,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.8666666666666667</v>
+        <v>0.91666666666666663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exceptions eliminiert. Program läuft auf meinem PC scheinbar nur noch widerwillig
</commit_message>
<xml_diff>
--- a/Checkliste Aufgabenstellung.xlsx
+++ b/Checkliste Aufgabenstellung.xlsx
@@ -507,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -932,7 +932,7 @@
       </c>
       <c r="D34" s="3">
         <f>SUM(D2:D33)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E34" s="3">
         <f>SUM(E2:E33)</f>
@@ -945,7 +945,7 @@
       </c>
       <c r="D35" s="4">
         <f>D34/60</f>
-        <v>0.91666666666666663</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>